<commit_message>
Added new packet marks and masks
</commit_message>
<xml_diff>
--- a/CES_Packet_Mark.xlsx
+++ b/CES_Packet_Mark.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="91">
   <si>
     <t>Direction</t>
   </si>
@@ -173,13 +173,130 @@
     <t>Egress Host to LEGACY  traffic MASK</t>
   </si>
   <si>
-    <t>Ingress CES from LOCAL traffic MASK</t>
-  </si>
-  <si>
-    <t>Egress CES to LOCAL traffic MASK - naah</t>
-  </si>
-  <si>
     <t>IDK</t>
+  </si>
+  <si>
+    <t>MARK_LOCAL_FROM_LAN</t>
+  </si>
+  <si>
+    <t>MARK_LOCAL_FROM_WAN</t>
+  </si>
+  <si>
+    <t>MARK_LOCAL_FROM_TUN</t>
+  </si>
+  <si>
+    <t>MARK_LAN_FROM_WAN</t>
+  </si>
+  <si>
+    <t>MARK_LAN_FROM_TUN</t>
+  </si>
+  <si>
+    <t>MARK_LOCAL_TO_LAN</t>
+  </si>
+  <si>
+    <t>MARK_LOCAL_TO_WAN</t>
+  </si>
+  <si>
+    <t>MARK_LOCAL_TO_TUN</t>
+  </si>
+  <si>
+    <t>MARK_LAN_TO_WAN</t>
+  </si>
+  <si>
+    <t>MARK_LAN_TO_TUN</t>
+  </si>
+  <si>
+    <t>Misc</t>
+  </si>
+  <si>
+    <t>MASK_LOCAL</t>
+  </si>
+  <si>
+    <t>MASK_LOCAL_INGRESS</t>
+  </si>
+  <si>
+    <t>MASK_LOCAL_EGRESS</t>
+  </si>
+  <si>
+    <t>Ingress LOCAL traffic MASK</t>
+  </si>
+  <si>
+    <t>Egress LOCAL traffic MASK - naah</t>
+  </si>
+  <si>
+    <t>MASK_HOST_LEGACY</t>
+  </si>
+  <si>
+    <t>MASK_HOST_CES</t>
+  </si>
+  <si>
+    <t>MASK_HOST_LEGACY_INGRESS</t>
+  </si>
+  <si>
+    <t>MASK_HOST_LEGACY_EGRESS</t>
+  </si>
+  <si>
+    <t>MASK_HOST_CES_INGRESS</t>
+  </si>
+  <si>
+    <t>MASK_HOST_CES_EGRESS</t>
+  </si>
+  <si>
+    <t>Ingress via LAN</t>
+  </si>
+  <si>
+    <t>Ingress via WAN</t>
+  </si>
+  <si>
+    <t>Ingress via TUN</t>
+  </si>
+  <si>
+    <t>MASK_LAN_INGRESS</t>
+  </si>
+  <si>
+    <t>MASK_WAN_INGRESS</t>
+  </si>
+  <si>
+    <t>MASK_TUN_INGRESS</t>
+  </si>
+  <si>
+    <t>MASK_LAN_EGRESS</t>
+  </si>
+  <si>
+    <t>MASK_WAN_EGRESS</t>
+  </si>
+  <si>
+    <t>MASK_TUN_EGRESS</t>
+  </si>
+  <si>
+    <t>Egress via LAN</t>
+  </si>
+  <si>
+    <t>Egress via WAN</t>
+  </si>
+  <si>
+    <t>Egress via TUN</t>
+  </si>
+  <si>
+    <t>MASK_HOST_INGRESS</t>
+  </si>
+  <si>
+    <t>MASK_HOST_EGRESS</t>
+  </si>
+  <si>
+    <t>Ingress HOST traffic MASK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egress HOST traffic MASK </t>
+  </si>
+  <si>
+    <t>Mask</t>
+  </si>
+  <si>
+    <t>FFFFFFFF</t>
+  </si>
+  <si>
+    <t>FF</t>
   </si>
 </sst>
 </file>
@@ -224,7 +341,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +409,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -362,7 +485,7 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,52 +529,70 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -737,319 +878,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N45"/>
+  <dimension ref="B2:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="7" width="18.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="38.5703125" style="1" customWidth="1"/>
-    <col min="10" max="13" width="18.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="9" width="18.5703125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="38.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" style="1" customWidth="1"/>
+    <col min="12" max="14" width="18.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="45.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="17">
-        <v>0</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="D4" s="15">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16">
         <f>$D$4</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
-      <c r="C5" s="20" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="20">
-        <v>1</v>
-      </c>
-      <c r="E5" s="18">
+      <c r="D5" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="16" t="str">
         <f>$D$5</f>
-        <v>1</v>
+        <v>FF</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="22">
-        <v>0</v>
-      </c>
-      <c r="E6" s="23">
+      <c r="D6" s="18">
+        <v>0</v>
+      </c>
+      <c r="E6" s="19">
         <f>$D$6</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="24"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="22">
-        <v>1</v>
-      </c>
-      <c r="E7" s="23">
+      <c r="D7" s="18">
+        <v>1</v>
+      </c>
+      <c r="E7" s="19">
         <f>$D$7</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="25"/>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="22">
-        <v>2</v>
-      </c>
-      <c r="E8" s="23">
+      <c r="D8" s="18">
+        <v>2</v>
+      </c>
+      <c r="E8" s="19">
         <f>$D$8</f>
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="20">
-        <v>0</v>
-      </c>
-      <c r="E9" s="18">
+      <c r="D9" s="17">
+        <v>0</v>
+      </c>
+      <c r="E9" s="16">
         <f>$D$9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="20">
-        <v>1</v>
-      </c>
-      <c r="E10" s="18">
+      <c r="D10" s="17">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
         <f>$D$10</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="19"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="20">
-        <v>2</v>
-      </c>
-      <c r="E11" s="18">
+      <c r="D11" s="17">
+        <v>2</v>
+      </c>
+      <c r="E11" s="16">
         <f>$D$11</f>
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="22">
-        <v>0</v>
-      </c>
-      <c r="E12" s="23">
+      <c r="D12" s="18">
+        <v>0</v>
+      </c>
+      <c r="E12" s="19">
         <f>$D$12</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="26"/>
+      <c r="C13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="22">
-        <v>1</v>
-      </c>
-      <c r="E13" s="23">
+      <c r="D13" s="18">
+        <v>1</v>
+      </c>
+      <c r="E13" s="19">
         <f>$D$13</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="24"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="22">
-        <v>2</v>
-      </c>
-      <c r="E14" s="23">
+      <c r="D14" s="18">
+        <v>2</v>
+      </c>
+      <c r="E14" s="19">
         <f>$D$14</f>
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="25"/>
-      <c r="C15" s="22" t="s">
+      <c r="B15" s="27"/>
+      <c r="C15" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="18">
         <v>3</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="19">
         <f>$D$15</f>
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="20">
-        <v>0</v>
-      </c>
-      <c r="E16" s="18">
+      <c r="D16" s="17">
+        <v>0</v>
+      </c>
+      <c r="E16" s="16">
         <f>$D$16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
-      <c r="C17" s="20" t="s">
+    <row r="17" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+      <c r="C17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="20">
-        <v>1</v>
-      </c>
-      <c r="E17" s="18">
+      <c r="D17" s="17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="16">
         <f>$D$17</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
-      <c r="C18" s="20" t="s">
+    <row r="18" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="22"/>
+      <c r="C18" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="20">
-        <v>2</v>
-      </c>
-      <c r="E18" s="18">
+      <c r="D18" s="17">
+        <v>2</v>
+      </c>
+      <c r="E18" s="16">
         <f>$D$18</f>
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
-      <c r="C19" s="20" t="s">
+    <row r="19" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="22"/>
+      <c r="C19" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="17">
         <v>3</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="16">
         <f>$D$19</f>
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="s">
+    <row r="20" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="23"/>
+      <c r="C20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="17">
         <v>4</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="16">
         <f>$D$20</f>
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
+    <row r="22" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="I22" s="15" t="s">
+      <c r="G22" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J22" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="K22" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="15" t="s">
+      <c r="L22" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="L22" s="15" t="s">
+      <c r="M22" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="15" t="s">
+      <c r="N22" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="N22" s="15" t="s">
+      <c r="O22" s="14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+      <c r="P22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="str">
         <f t="shared" ref="B23:B32" si="0">$D$5</f>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C23" s="2">
         <f>$D$7</f>
@@ -1076,29 +1223,38 @@
         <v>2</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2" t="str">
+      <c r="K23" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="L23" s="2" t="str">
         <f>CONCATENATE("0x",B23,C23,D23,E23,F23,G23,H23)</f>
-        <v>0x1121212</v>
-      </c>
-      <c r="L23" s="2" t="str">
+        <v>0xFF121212</v>
+      </c>
+      <c r="M23" s="2" t="str">
         <f>CONCATENATE(B23,C23,D23,E23,F23,G23,H23)</f>
-        <v>1121212</v>
-      </c>
-      <c r="M23" s="3">
-        <f>HEX2DEC(L23)</f>
-        <v>17961490</v>
-      </c>
-      <c r="N23" s="12" t="s">
+        <v>FF121212</v>
+      </c>
+      <c r="N23" s="3">
+        <f>HEX2DEC(M23)</f>
+        <v>4279374354</v>
+      </c>
+      <c r="O23" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
+      <c r="P23" s="28" t="str">
+        <f>CONCATENATE(K23,"=",CHAR(34),L23,CHAR(34))</f>
+        <v>MARK_LOCAL_FROM_LAN="0xFF121212"</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C24" s="2">
         <f>$D$8</f>
@@ -1125,32 +1281,41 @@
         <v>1</v>
       </c>
       <c r="I24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2" t="str">
-        <f t="shared" ref="K24:K32" si="2">CONCATENATE("0x",B24,C24,D24,E24,F24,G24,H24)</f>
-        <v>0x1211221</v>
+      <c r="K24" s="29" t="s">
+        <v>55</v>
       </c>
       <c r="L24" s="2" t="str">
-        <f t="shared" ref="L24:L32" si="3">CONCATENATE(B24,C24,D24,E24,F24,G24,H24)</f>
-        <v>1211221</v>
-      </c>
-      <c r="M24" s="3">
-        <f t="shared" ref="M24:M31" si="4">HEX2DEC(L24)</f>
-        <v>18944545</v>
-      </c>
-      <c r="N24" s="13" t="s">
+        <f t="shared" ref="L24:L32" si="2">CONCATENATE("0x",B24,C24,D24,E24,F24,G24,H24)</f>
+        <v>0xFF211221</v>
+      </c>
+      <c r="M24" s="2" t="str">
+        <f t="shared" ref="M24:M32" si="3">CONCATENATE(B24,C24,D24,E24,F24,G24,H24)</f>
+        <v>FF211221</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" ref="N24:N31" si="4">HEX2DEC(M24)</f>
+        <v>4280357409</v>
+      </c>
+      <c r="O24" s="13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
+      <c r="P24" s="28" t="str">
+        <f t="shared" ref="P24:P32" si="5">CONCATENATE(K24,"=",CHAR(34),L24,CHAR(34))</f>
+        <v>MARK_LOCAL_TO_LAN="0xFF211221"</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C25" s="4">
-        <f t="shared" ref="C25:C28" si="5">$D$6</f>
+        <f t="shared" ref="C25:C28" si="6">$D$6</f>
         <v>0</v>
       </c>
       <c r="D25" s="4">
@@ -1174,32 +1339,41 @@
         <v>3</v>
       </c>
       <c r="I25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4" t="str">
+      <c r="K25" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="L25" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>0x1021113</v>
-      </c>
-      <c r="L25" s="4" t="str">
+        <v>0xFF021113</v>
+      </c>
+      <c r="M25" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>1021113</v>
-      </c>
-      <c r="M25" s="5">
+        <v>FF021113</v>
+      </c>
+      <c r="N25" s="5">
         <f t="shared" si="4"/>
-        <v>16912659</v>
-      </c>
-      <c r="N25" s="12" t="s">
+        <v>4278325523</v>
+      </c>
+      <c r="O25" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="26" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
+      <c r="P25" s="28" t="str">
+        <f t="shared" si="5"/>
+        <v>MARK_LOCAL_FROM_WAN="0xFF021113"</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C26" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D26" s="4">
@@ -1223,32 +1397,41 @@
         <v>1</v>
       </c>
       <c r="I26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4" t="str">
+      <c r="K26" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="L26" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>0x1011131</v>
-      </c>
-      <c r="L26" s="4" t="str">
+        <v>0xFF011131</v>
+      </c>
+      <c r="M26" s="4" t="str">
         <f t="shared" si="3"/>
-        <v>1011131</v>
-      </c>
-      <c r="M26" s="5">
+        <v>FF011131</v>
+      </c>
+      <c r="N26" s="5">
         <f t="shared" si="4"/>
-        <v>16847153</v>
-      </c>
-      <c r="N26" s="13" t="s">
+        <v>4278260017</v>
+      </c>
+      <c r="O26" s="13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="6">
+      <c r="P26" s="28" t="str">
+        <f t="shared" si="5"/>
+        <v>MARK_LOCAL_TO_WAN="0xFF011131"</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C27" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D27" s="6">
@@ -1272,32 +1455,41 @@
         <v>4</v>
       </c>
       <c r="I27" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6" t="str">
+      <c r="K27" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="L27" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>0x1021114</v>
-      </c>
-      <c r="L27" s="6" t="str">
+        <v>0xFF021114</v>
+      </c>
+      <c r="M27" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>1021114</v>
-      </c>
-      <c r="M27" s="7">
+        <v>FF021114</v>
+      </c>
+      <c r="N27" s="7">
         <f t="shared" si="4"/>
-        <v>16912660</v>
-      </c>
-      <c r="N27" s="12" t="s">
+        <v>4278325524</v>
+      </c>
+      <c r="O27" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="6">
+      <c r="P27" s="28" t="str">
+        <f t="shared" si="5"/>
+        <v>MARK_LOCAL_FROM_TUN="0xFF021114"</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C28" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D28" s="6">
@@ -1321,29 +1513,38 @@
         <v>1</v>
       </c>
       <c r="I28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6" t="str">
+      <c r="K28" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="L28" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>0x1011141</v>
-      </c>
-      <c r="L28" s="6" t="str">
+        <v>0xFF011141</v>
+      </c>
+      <c r="M28" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>1011141</v>
-      </c>
-      <c r="M28" s="7">
+        <v>FF011141</v>
+      </c>
+      <c r="N28" s="7">
         <f t="shared" si="4"/>
-        <v>16847169</v>
-      </c>
-      <c r="N28" s="13" t="s">
+        <v>4278260033</v>
+      </c>
+      <c r="O28" s="13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="8">
+      <c r="P28" s="28" t="str">
+        <f t="shared" si="5"/>
+        <v>MARK_LOCAL_TO_TUN="0xFF011141"</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C29" s="8">
         <f>$D$8</f>
@@ -1354,7 +1555,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="8">
-        <f t="shared" ref="E29:E32" si="6">$D$11</f>
+        <f t="shared" ref="E29:E32" si="7">$D$11</f>
         <v>2</v>
       </c>
       <c r="F29" s="8">
@@ -1370,29 +1571,38 @@
         <v>3</v>
       </c>
       <c r="I29" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8" t="str">
+      <c r="K29" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="L29" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>0x1222223</v>
-      </c>
-      <c r="L29" s="8" t="str">
+        <v>0xFF222223</v>
+      </c>
+      <c r="M29" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>1222223</v>
-      </c>
-      <c r="M29" s="9">
+        <v>FF222223</v>
+      </c>
+      <c r="N29" s="9">
         <f t="shared" si="4"/>
-        <v>19014179</v>
-      </c>
-      <c r="N29" s="12" t="s">
+        <v>4280427043</v>
+      </c>
+      <c r="O29" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="8">
+      <c r="P29" s="28" t="str">
+        <f t="shared" si="5"/>
+        <v>MARK_LAN_TO_WAN="0xFF222223"</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C30" s="8">
         <f>$D$7</f>
@@ -1419,29 +1629,38 @@
         <v>2</v>
       </c>
       <c r="I30" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8" t="str">
+      <c r="K30" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="L30" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>0x1112232</v>
-      </c>
-      <c r="L30" s="8" t="str">
+        <v>0xFF112232</v>
+      </c>
+      <c r="M30" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>1112232</v>
-      </c>
-      <c r="M30" s="9">
-        <f>HEX2DEC(L30)</f>
-        <v>17900082</v>
-      </c>
-      <c r="N30" s="12" t="s">
+        <v>FF112232</v>
+      </c>
+      <c r="N30" s="9">
+        <f>HEX2DEC(M30)</f>
+        <v>4279312946</v>
+      </c>
+      <c r="O30" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="10">
+      <c r="P30" s="28" t="str">
+        <f t="shared" si="5"/>
+        <v>MARK_LAN_FROM_WAN="0xFF112232"</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C31" s="11">
         <f>$D$8</f>
@@ -1452,7 +1671,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="F31" s="10">
@@ -1468,29 +1687,38 @@
         <v>2</v>
       </c>
       <c r="I31" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="J31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10" t="str">
+      <c r="K31" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="L31" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>0x1222342</v>
-      </c>
-      <c r="L31" s="10" t="str">
+        <v>0xFF222342</v>
+      </c>
+      <c r="M31" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>1222342</v>
-      </c>
-      <c r="M31" s="11">
+        <v>FF222342</v>
+      </c>
+      <c r="N31" s="11">
         <f t="shared" si="4"/>
-        <v>19014466</v>
-      </c>
-      <c r="N31" s="12" t="s">
+        <v>4280427330</v>
+      </c>
+      <c r="O31" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="10">
+      <c r="P31" s="28" t="str">
+        <f t="shared" si="5"/>
+        <v>MARK_LAN_TO_TUN="0xFF222342"</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>FF</v>
       </c>
       <c r="C32" s="11">
         <f>$D$7</f>
@@ -1501,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="F32" s="10">
@@ -1516,462 +1744,1056 @@
         <f>$D$20</f>
         <v>4</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="J32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10" t="str">
+      <c r="K32" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="L32" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>0x1112324</v>
-      </c>
-      <c r="L32" s="10" t="str">
+        <v>0xFF112324</v>
+      </c>
+      <c r="M32" s="10" t="str">
         <f t="shared" si="3"/>
-        <v>1112324</v>
-      </c>
-      <c r="M32" s="11">
-        <f>HEX2DEC(L32)</f>
-        <v>17900324</v>
-      </c>
-      <c r="N32" s="12" t="s">
+        <v>FF112324</v>
+      </c>
+      <c r="N32" s="11">
+        <f>HEX2DEC(M32)</f>
+        <v>4279313188</v>
+      </c>
+      <c r="O32" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="35" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="27">
-        <f t="shared" ref="B35:B45" si="7">$D$5</f>
-        <v>1</v>
-      </c>
-      <c r="C35" s="29">
-        <f t="shared" ref="C35:C37" si="8">$D$6</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="27">
+      <c r="P32" s="28" t="str">
+        <f t="shared" si="5"/>
+        <v>MARK_LAN_FROM_TUN="0xFF112324"</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="28"/>
+      <c r="P33" s="28"/>
+    </row>
+    <row r="34" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="28"/>
+      <c r="P34" s="28"/>
+    </row>
+    <row r="35" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="34" t="str">
+        <f t="shared" ref="B35:B55" si="8">$D$5</f>
+        <v>FF</v>
+      </c>
+      <c r="C35" s="34">
+        <f t="shared" ref="C35:D40" si="9">$D$6</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="34">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E35" s="27">
-        <f t="shared" ref="E35:E37" si="9">$D$10</f>
-        <v>1</v>
-      </c>
-      <c r="F35" s="27">
+      <c r="E35" s="34">
+        <f t="shared" ref="E35:E37" si="10">$D$10</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="34">
         <f>$D$12</f>
         <v>0</v>
       </c>
-      <c r="G35" s="27">
-        <f t="shared" ref="G35:G37" si="10">$D$17</f>
-        <v>1</v>
-      </c>
-      <c r="H35" s="27">
+      <c r="G35" s="34">
+        <f t="shared" ref="G35:H40" si="11">$D$17</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="34">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="I35" s="28" t="s">
+      <c r="I35" s="34" t="str">
+        <f>CONCATENATE(IF(B35&lt;&gt;0,"FF","0"),IF(C35&lt;&gt;0,"F","0"),IF(D35&lt;&gt;0,"F","0"), IF(E35&lt;&gt;0,"F","0"),IF(F35&lt;&gt;0,"F","0"),IF(G35&lt;&gt;0,"F","0"), IF(H35&lt;&gt;0,"F","0"))</f>
+        <v>FF00F0F0</v>
+      </c>
+      <c r="J35" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="K35" s="10" t="str">
-        <f t="shared" ref="K35" si="11">CONCATENATE("0x",B35,C35,D35,E35,F35,G35,H35)</f>
-        <v>0x1001010</v>
-      </c>
-      <c r="L35" s="10" t="str">
-        <f t="shared" ref="L35" si="12">CONCATENATE(B35,C35,D35,E35,F35,G35,H35)</f>
-        <v>1001010</v>
-      </c>
-      <c r="M35" s="11">
-        <f>HEX2DEC(L35)</f>
-        <v>16781328</v>
-      </c>
-      <c r="N35" s="30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="27">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="C36" s="29">
+      <c r="K35" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="L35" s="35" t="str">
+        <f t="shared" ref="L35" si="12">CONCATENATE("0x",B35,C35,D35,E35,F35,G35,H35)</f>
+        <v>0xFF001010</v>
+      </c>
+      <c r="M35" s="35" t="str">
+        <f t="shared" ref="M35" si="13">CONCATENATE(B35,C35,D35,E35,F35,G35,H35)</f>
+        <v>FF001010</v>
+      </c>
+      <c r="N35" s="36">
+        <f>HEX2DEC(M35)</f>
+        <v>4278194192</v>
+      </c>
+      <c r="O35" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="P35" s="28" t="str">
+        <f>CONCATENATE(K35,"=",CHAR(34),L35,"/0x",I35,CHAR(34))</f>
+        <v>MASK_LOCAL="0xFF001010/0xFF00F0F0"</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="34" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D36" s="27">
+        <v>FF</v>
+      </c>
+      <c r="C36" s="34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D36" s="34">
         <f>$D$8</f>
         <v>2</v>
       </c>
-      <c r="E36" s="27">
+      <c r="E36" s="34">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="F36" s="34">
+        <f>$D$12</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="34">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="H36" s="34">
+        <f t="shared" ref="G36:H47" si="14">$D$16</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="34" t="str">
+        <f t="shared" ref="I36:I37" si="15">CONCATENATE(IF(B36&lt;&gt;0,"FF","0"),IF(C36&lt;&gt;0,"F","0"),IF(D36&lt;&gt;0,"F","0"), IF(E36&lt;&gt;0,"F","0"),IF(F36&lt;&gt;0,"F","0"),IF(G36&lt;&gt;0,"F","0"), IF(H36&lt;&gt;0,"F","0"))</f>
+        <v>FF0FF0F0</v>
+      </c>
+      <c r="J36" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="K36" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="L36" s="35" t="str">
+        <f t="shared" ref="L36:L37" si="16">CONCATENATE("0x",B36,C36,D36,E36,F36,G36,H36)</f>
+        <v>0xFF021010</v>
+      </c>
+      <c r="M36" s="35" t="str">
+        <f t="shared" ref="M36:M37" si="17">CONCATENATE(B36,C36,D36,E36,F36,G36,H36)</f>
+        <v>FF021010</v>
+      </c>
+      <c r="N36" s="36">
+        <f t="shared" ref="N36:N37" si="18">HEX2DEC(M36)</f>
+        <v>4278325264</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P36" s="28" t="str">
+        <f t="shared" ref="P36:P55" si="19">CONCATENATE(K36,"=",CHAR(34),L36,"/0x",I36,CHAR(34))</f>
+        <v>MASK_LOCAL_INGRESS="0xFF021010/0xFF0FF0F0"</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C37" s="34">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="F36" s="27">
+        <v>0</v>
+      </c>
+      <c r="D37" s="34">
+        <f>$D$7</f>
+        <v>1</v>
+      </c>
+      <c r="E37" s="34">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="F37" s="34">
         <f>$D$12</f>
         <v>0</v>
       </c>
-      <c r="G36" s="27">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="H36" s="27">
-        <f t="shared" ref="H36:H44" si="13">$D$16</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="K36" s="10" t="str">
-        <f t="shared" ref="K36:K37" si="14">CONCATENATE("0x",B36,C36,D36,E36,F36,G36,H36)</f>
-        <v>0x1021010</v>
-      </c>
-      <c r="L36" s="10" t="str">
-        <f t="shared" ref="L36:L37" si="15">CONCATENATE(B36,C36,D36,E36,F36,G36,H36)</f>
-        <v>1021010</v>
-      </c>
-      <c r="M36" s="11">
-        <f t="shared" ref="M36:M37" si="16">HEX2DEC(L36)</f>
-        <v>16912400</v>
-      </c>
-      <c r="N36" s="12" t="s">
+      <c r="G37" s="34">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="34">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="I37" s="34" t="str">
+        <f t="shared" si="15"/>
+        <v>FF0FF00F</v>
+      </c>
+      <c r="J37" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="K37" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="L37" s="35" t="str">
+        <f t="shared" si="16"/>
+        <v>0xFF011001</v>
+      </c>
+      <c r="M37" s="35" t="str">
+        <f t="shared" si="17"/>
+        <v>FF011001</v>
+      </c>
+      <c r="N37" s="36">
+        <f t="shared" si="18"/>
+        <v>4278259713</v>
+      </c>
+      <c r="O37" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="P37" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_LOCAL_EGRESS="0xFF011001/0xFF0FF00F"</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P38" s="28"/>
+    </row>
+    <row r="39" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C39" s="34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="D39" s="34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="34">
+        <f t="shared" ref="E39:E40" si="20">$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="34">
+        <f>$D$12</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="34">
+        <f>$D$18</f>
+        <v>2</v>
+      </c>
+      <c r="H39" s="34">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="34" t="str">
+        <f t="shared" ref="I39:I40" si="21">CONCATENATE(IF(B39&lt;&gt;0,"FF","0"),IF(C39&lt;&gt;0,"F","0"),IF(D39&lt;&gt;0,"F","0"), IF(E39&lt;&gt;0,"F","0"),IF(F39&lt;&gt;0,"F","0"),IF(G39&lt;&gt;0,"F","0"), IF(H39&lt;&gt;0,"F","0"))</f>
+        <v>FF0000F0</v>
+      </c>
+      <c r="J39" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="K39" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="L39" s="35" t="str">
+        <f>CONCATENATE("0x",B39,C39,D39,E39,F39,G39,H39)</f>
+        <v>0xFF000020</v>
+      </c>
+      <c r="M39" s="35" t="str">
+        <f>CONCATENATE(B39,C39,D39,E39,F39,G39,H39)</f>
+        <v>FF000020</v>
+      </c>
+      <c r="N39" s="36">
+        <f t="shared" ref="N39:N40" si="22">HEX2DEC(M39)</f>
+        <v>4278190112</v>
+      </c>
+      <c r="O39" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="27">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="C37" s="29">
+      <c r="P39" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_HOST_INGRESS="0xFF000020/0xFF0000F0"</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="34" t="str">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="D37" s="27">
-        <f>$D$7</f>
-        <v>1</v>
-      </c>
-      <c r="E37" s="27">
+        <v>FF</v>
+      </c>
+      <c r="C40" s="34">
         <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="F37" s="27">
+        <v>0</v>
+      </c>
+      <c r="D40" s="34">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="34">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="34">
         <f>$D$12</f>
         <v>0</v>
       </c>
-      <c r="G37" s="27">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="H37" s="27">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="K37" s="10" t="str">
+      <c r="G40" s="34">
         <f t="shared" si="14"/>
-        <v>0x1011010</v>
-      </c>
-      <c r="L37" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>1011010</v>
-      </c>
-      <c r="M37" s="11">
-        <f t="shared" si="16"/>
-        <v>16846864</v>
-      </c>
-      <c r="N37" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N38"/>
-    </row>
-    <row r="39" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="27">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="C39" s="29">
-        <f t="shared" ref="C39:C45" si="17">$D$6</f>
-        <v>0</v>
-      </c>
-      <c r="D39" s="27">
+        <v>0</v>
+      </c>
+      <c r="H40" s="34">
+        <f>$D$18</f>
+        <v>2</v>
+      </c>
+      <c r="I40" s="34" t="str">
+        <f t="shared" si="21"/>
+        <v>FF00000F</v>
+      </c>
+      <c r="J40" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="K40" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="L40" s="35" t="str">
+        <f>CONCATENATE("0x",B40,C40,D40,E40,F40,G40,H40)</f>
+        <v>0xFF000002</v>
+      </c>
+      <c r="M40" s="35" t="str">
+        <f>CONCATENATE(B40,C40,D40,E40,F40,G40,H40)</f>
+        <v>FF000002</v>
+      </c>
+      <c r="N40" s="36">
+        <f t="shared" si="22"/>
+        <v>4278190082</v>
+      </c>
+      <c r="O40" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P40" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_HOST_EGRESS="0xFF000002/0xFF00000F"</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P41" s="28"/>
+    </row>
+    <row r="42" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C42" s="34">
+        <f t="shared" ref="C42:D55" si="23">$D$6</f>
+        <v>0</v>
+      </c>
+      <c r="D42" s="34">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E39" s="27">
+      <c r="E42" s="34">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F42" s="34">
         <f>$D$14</f>
         <v>2</v>
       </c>
-      <c r="G39" s="27">
+      <c r="G42" s="34">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H39" s="27">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I39" s="28" t="s">
+      <c r="H42" s="34">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I42" s="34" t="str">
+        <f t="shared" ref="I42:I44" si="24">CONCATENATE(IF(B42&lt;&gt;0,"FF","0"),IF(C42&lt;&gt;0,"F","0"),IF(D42&lt;&gt;0,"F","0"), IF(E42&lt;&gt;0,"F","0"),IF(F42&lt;&gt;0,"F","0"),IF(G42&lt;&gt;0,"F","0"), IF(H42&lt;&gt;0,"F","0"))</f>
+        <v>FF000F00</v>
+      </c>
+      <c r="J42" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="K39" s="10" t="str">
-        <f t="shared" ref="K39" si="18">CONCATENATE("0x",B39,C39,D39,E39,F39,G39,H39)</f>
-        <v>0x1000200</v>
-      </c>
-      <c r="L39" s="10" t="str">
-        <f t="shared" ref="L39" si="19">CONCATENATE(B39,C39,D39,E39,F39,G39,H39)</f>
-        <v>1000200</v>
-      </c>
-      <c r="M39" s="11">
-        <f>HEX2DEC(L39)</f>
-        <v>16777728</v>
-      </c>
-      <c r="N39" s="12" t="s">
+      <c r="K42" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="L42" s="35" t="str">
+        <f t="shared" ref="L42" si="25">CONCATENATE("0x",B42,C42,D42,E42,F42,G42,H42)</f>
+        <v>0xFF000200</v>
+      </c>
+      <c r="M42" s="35" t="str">
+        <f t="shared" ref="M42" si="26">CONCATENATE(B42,C42,D42,E42,F42,G42,H42)</f>
+        <v>FF000200</v>
+      </c>
+      <c r="N42" s="36">
+        <f>HEX2DEC(M42)</f>
+        <v>4278190592</v>
+      </c>
+      <c r="O42" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="27">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="C40" s="29">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="D40" s="27">
+      <c r="P42" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_HOST_LEGACY="0xFF000200/0xFF000F00"</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C43" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D43" s="34">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E40" s="27">
+      <c r="E43" s="34">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F40" s="23">
+      <c r="F43" s="34">
         <f>$D$14</f>
         <v>2</v>
       </c>
-      <c r="G40" s="27">
+      <c r="G43" s="34">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="H40" s="27">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I40" s="28" t="s">
+      <c r="H43" s="34">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="34" t="str">
+        <f t="shared" si="24"/>
+        <v>FF000FF0</v>
+      </c>
+      <c r="J43" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="K40" s="10" t="str">
-        <f t="shared" ref="K40:K41" si="20">CONCATENATE("0x",B40,C40,D40,E40,F40,G40,H40)</f>
-        <v>0x1000220</v>
-      </c>
-      <c r="L40" s="10" t="str">
-        <f t="shared" ref="L40:L41" si="21">CONCATENATE(B40,C40,D40,E40,F40,G40,H40)</f>
-        <v>1000220</v>
-      </c>
-      <c r="M40" s="11">
-        <f t="shared" ref="M40:M41" si="22">HEX2DEC(L40)</f>
-        <v>16777760</v>
-      </c>
-      <c r="N40" s="12" t="s">
+      <c r="K43" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="L43" s="35" t="str">
+        <f t="shared" ref="L43:L44" si="27">CONCATENATE("0x",B43,C43,D43,E43,F43,G43,H43)</f>
+        <v>0xFF000220</v>
+      </c>
+      <c r="M43" s="35" t="str">
+        <f t="shared" ref="M43:M44" si="28">CONCATENATE(B43,C43,D43,E43,F43,G43,H43)</f>
+        <v>FF000220</v>
+      </c>
+      <c r="N43" s="36">
+        <f t="shared" ref="N43:N44" si="29">HEX2DEC(M43)</f>
+        <v>4278190624</v>
+      </c>
+      <c r="O43" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="27">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="C41" s="29">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="D41" s="27">
+      <c r="P43" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_HOST_LEGACY_INGRESS="0xFF000220/0xFF000FF0"</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C44" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D44" s="34">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E41" s="27">
+      <c r="E44" s="34">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F41" s="23">
+      <c r="F44" s="34">
         <f>$D$14</f>
         <v>2</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G44" s="34">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H41" s="27">
+      <c r="H44" s="34">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="I41" s="28" t="s">
+      <c r="I44" s="34" t="str">
+        <f t="shared" si="24"/>
+        <v>FF000F0F</v>
+      </c>
+      <c r="J44" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="K41" s="10" t="str">
-        <f t="shared" si="20"/>
-        <v>0x1000202</v>
-      </c>
-      <c r="L41" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>1000202</v>
-      </c>
-      <c r="M41" s="11">
-        <f t="shared" si="22"/>
-        <v>16777730</v>
-      </c>
-      <c r="N41" s="12" t="s">
+      <c r="K44" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="L44" s="35" t="str">
+        <f t="shared" si="27"/>
+        <v>0xFF000202</v>
+      </c>
+      <c r="M44" s="35" t="str">
+        <f t="shared" si="28"/>
+        <v>FF000202</v>
+      </c>
+      <c r="N44" s="36">
+        <f t="shared" si="29"/>
+        <v>4278190594</v>
+      </c>
+      <c r="O44" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N42"/>
-    </row>
-    <row r="43" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="27">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="C43" s="29">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="D43" s="27">
+      <c r="P44" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_HOST_LEGACY_EGRESS="0xFF000202/0xFF000F0F"</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P45" s="28"/>
+    </row>
+    <row r="46" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C46" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D46" s="34">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E43" s="27">
+      <c r="E46" s="34">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F46" s="34">
         <f>$D$15</f>
         <v>3</v>
       </c>
-      <c r="G43" s="27">
+      <c r="G46" s="34">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H43" s="27">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I43" s="28" t="s">
+      <c r="H46" s="34">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I46" s="34" t="str">
+        <f t="shared" ref="I46:I48" si="30">CONCATENATE(IF(B46&lt;&gt;0,"FF","0"),IF(C46&lt;&gt;0,"F","0"),IF(D46&lt;&gt;0,"F","0"), IF(E46&lt;&gt;0,"F","0"),IF(F46&lt;&gt;0,"F","0"),IF(G46&lt;&gt;0,"F","0"), IF(H46&lt;&gt;0,"F","0"))</f>
+        <v>FF000F00</v>
+      </c>
+      <c r="J46" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="K43" s="10" t="str">
-        <f t="shared" ref="K43" si="23">CONCATENATE("0x",B43,C43,D43,E43,F43,G43,H43)</f>
-        <v>0x1000300</v>
-      </c>
-      <c r="L43" s="10" t="str">
-        <f t="shared" ref="L43" si="24">CONCATENATE(B43,C43,D43,E43,F43,G43,H43)</f>
-        <v>1000300</v>
-      </c>
-      <c r="M43" s="11">
-        <f>HEX2DEC(L43)</f>
-        <v>16777984</v>
-      </c>
-      <c r="N43" s="12" t="s">
+      <c r="K46" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="L46" s="35" t="str">
+        <f t="shared" ref="L46" si="31">CONCATENATE("0x",B46,C46,D46,E46,F46,G46,H46)</f>
+        <v>0xFF000300</v>
+      </c>
+      <c r="M46" s="35" t="str">
+        <f t="shared" ref="M46" si="32">CONCATENATE(B46,C46,D46,E46,F46,G46,H46)</f>
+        <v>FF000300</v>
+      </c>
+      <c r="N46" s="36">
+        <f>HEX2DEC(M46)</f>
+        <v>4278190848</v>
+      </c>
+      <c r="O46" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="44" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="27">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="C44" s="29">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="D44" s="27">
+      <c r="P46" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_HOST_CES="0xFF000300/0xFF000F00"</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C47" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D47" s="34">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E44" s="27">
+      <c r="E47" s="34">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F44" s="23">
-        <f t="shared" ref="F44:F45" si="25">$D$15</f>
+      <c r="F47" s="34">
+        <f t="shared" ref="F47:F48" si="33">$D$15</f>
         <v>3</v>
       </c>
-      <c r="G44" s="27">
+      <c r="G47" s="34">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="H44" s="27">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="I44" s="28" t="s">
+      <c r="H47" s="34">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="34" t="str">
+        <f t="shared" si="30"/>
+        <v>FF000FF0</v>
+      </c>
+      <c r="J47" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="K44" s="10" t="str">
-        <f t="shared" ref="K44:K45" si="26">CONCATENATE("0x",B44,C44,D44,E44,F44,G44,H44)</f>
-        <v>0x1000320</v>
-      </c>
-      <c r="L44" s="10" t="str">
-        <f t="shared" ref="L44:L45" si="27">CONCATENATE(B44,C44,D44,E44,F44,G44,H44)</f>
-        <v>1000320</v>
-      </c>
-      <c r="M44" s="11">
-        <f t="shared" ref="M44:M45" si="28">HEX2DEC(L44)</f>
-        <v>16778016</v>
-      </c>
-      <c r="N44" s="12" t="s">
+      <c r="K47" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="L47" s="35" t="str">
+        <f t="shared" ref="L47:L48" si="34">CONCATENATE("0x",B47,C47,D47,E47,F47,G47,H47)</f>
+        <v>0xFF000320</v>
+      </c>
+      <c r="M47" s="35" t="str">
+        <f t="shared" ref="M47:M48" si="35">CONCATENATE(B47,C47,D47,E47,F47,G47,H47)</f>
+        <v>FF000320</v>
+      </c>
+      <c r="N47" s="36">
+        <f t="shared" ref="N47:N48" si="36">HEX2DEC(M47)</f>
+        <v>4278190880</v>
+      </c>
+      <c r="O47" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="2:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="27">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="C45" s="29">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="D45" s="27">
+      <c r="P47" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_HOST_CES_INGRESS="0xFF000320/0xFF000FF0"</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C48" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D48" s="34">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E45" s="27">
+      <c r="E48" s="34">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F45" s="23">
-        <f t="shared" si="25"/>
+      <c r="F48" s="34">
+        <f t="shared" si="33"/>
         <v>3</v>
       </c>
-      <c r="G45" s="27">
+      <c r="G48" s="34">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H45" s="27">
+      <c r="H48" s="34">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="I45" s="28" t="s">
+      <c r="I48" s="34" t="str">
+        <f t="shared" si="30"/>
+        <v>FF000F0F</v>
+      </c>
+      <c r="J48" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="K45" s="10" t="str">
-        <f t="shared" si="26"/>
-        <v>0x1000302</v>
-      </c>
-      <c r="L45" s="10" t="str">
-        <f t="shared" si="27"/>
-        <v>1000302</v>
-      </c>
-      <c r="M45" s="11">
-        <f t="shared" si="28"/>
-        <v>16777986</v>
-      </c>
-      <c r="N45" s="12" t="s">
+      <c r="K48" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="L48" s="35" t="str">
+        <f t="shared" si="34"/>
+        <v>0xFF000302</v>
+      </c>
+      <c r="M48" s="35" t="str">
+        <f t="shared" si="35"/>
+        <v>FF000302</v>
+      </c>
+      <c r="N48" s="36">
+        <f t="shared" si="36"/>
+        <v>4278190850</v>
+      </c>
+      <c r="O48" s="12" t="s">
         <v>39</v>
+      </c>
+      <c r="P48" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_HOST_CES_EGRESS="0xFF000302/0xFF000F0F"</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P49" s="28"/>
+    </row>
+    <row r="50" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C50" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D50" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="E50" s="34">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="34">
+        <f>$D$12</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="34">
+        <f>$D$16</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="34">
+        <f>$D$18</f>
+        <v>2</v>
+      </c>
+      <c r="I50" s="34" t="str">
+        <f t="shared" ref="I50:I55" si="37">CONCATENATE(IF(B50&lt;&gt;0,"FF","0"),IF(C50&lt;&gt;0,"F","0"),IF(D50&lt;&gt;0,"F","0"), IF(E50&lt;&gt;0,"F","0"),IF(F50&lt;&gt;0,"F","0"),IF(G50&lt;&gt;0,"F","0"), IF(H50&lt;&gt;0,"F","0"))</f>
+        <v>FF00000F</v>
+      </c>
+      <c r="J50" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="K50" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="L50" s="35" t="str">
+        <f t="shared" ref="L50" si="38">CONCATENATE("0x",B50,C50,D50,E50,F50,G50,H50)</f>
+        <v>0xFF000002</v>
+      </c>
+      <c r="M50" s="35" t="str">
+        <f t="shared" ref="M50" si="39">CONCATENATE(B50,C50,D50,E50,F50,G50,H50)</f>
+        <v>FF000002</v>
+      </c>
+      <c r="N50" s="36">
+        <f t="shared" ref="N50" si="40">HEX2DEC(M50)</f>
+        <v>4278190082</v>
+      </c>
+      <c r="O50" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P50" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_LAN_INGRESS="0xFF000002/0xFF00000F"</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C51" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D51" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="E51" s="34">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="34">
+        <f>$D$12</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="34">
+        <f>$D$16</f>
+        <v>0</v>
+      </c>
+      <c r="H51" s="34">
+        <f>$D$19</f>
+        <v>3</v>
+      </c>
+      <c r="I51" s="34" t="str">
+        <f t="shared" si="37"/>
+        <v>FF00000F</v>
+      </c>
+      <c r="J51" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="K51" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="L51" s="35" t="str">
+        <f t="shared" ref="L51:L55" si="41">CONCATENATE("0x",B51,C51,D51,E51,F51,G51,H51)</f>
+        <v>0xFF000003</v>
+      </c>
+      <c r="M51" s="35" t="str">
+        <f t="shared" ref="M51:M55" si="42">CONCATENATE(B51,C51,D51,E51,F51,G51,H51)</f>
+        <v>FF000003</v>
+      </c>
+      <c r="N51" s="36">
+        <f t="shared" ref="N51:N55" si="43">HEX2DEC(M51)</f>
+        <v>4278190083</v>
+      </c>
+      <c r="O51" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P51" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_WAN_INGRESS="0xFF000003/0xFF00000F"</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C52" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D52" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="E52" s="34">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="F52" s="34">
+        <f>$D$12</f>
+        <v>0</v>
+      </c>
+      <c r="G52" s="34">
+        <f>$D$16</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="34">
+        <f>$D$20</f>
+        <v>4</v>
+      </c>
+      <c r="I52" s="34" t="str">
+        <f t="shared" si="37"/>
+        <v>FF00000F</v>
+      </c>
+      <c r="J52" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K52" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="L52" s="35" t="str">
+        <f t="shared" si="41"/>
+        <v>0xFF000004</v>
+      </c>
+      <c r="M52" s="35" t="str">
+        <f t="shared" si="42"/>
+        <v>FF000004</v>
+      </c>
+      <c r="N52" s="36">
+        <f t="shared" si="43"/>
+        <v>4278190084</v>
+      </c>
+      <c r="O52" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="P52" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_TUN_INGRESS="0xFF000004/0xFF00000F"</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C53" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D53" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="E53" s="34">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="34">
+        <f>$D$12</f>
+        <v>0</v>
+      </c>
+      <c r="G53" s="34">
+        <f>$D$18</f>
+        <v>2</v>
+      </c>
+      <c r="H53" s="34">
+        <f>$D$16</f>
+        <v>0</v>
+      </c>
+      <c r="I53" s="34" t="str">
+        <f t="shared" si="37"/>
+        <v>FF0000F0</v>
+      </c>
+      <c r="J53" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="K53" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="L53" s="35" t="str">
+        <f t="shared" si="41"/>
+        <v>0xFF000020</v>
+      </c>
+      <c r="M53" s="35" t="str">
+        <f t="shared" si="42"/>
+        <v>FF000020</v>
+      </c>
+      <c r="N53" s="36">
+        <f t="shared" si="43"/>
+        <v>4278190112</v>
+      </c>
+      <c r="O53" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="P53" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_LAN_EGRESS="0xFF000020/0xFF0000F0"</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C54" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D54" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="E54" s="34">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="F54" s="34">
+        <f>$D$12</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="34">
+        <f>$D$19</f>
+        <v>3</v>
+      </c>
+      <c r="H54" s="34">
+        <f>$D$16</f>
+        <v>0</v>
+      </c>
+      <c r="I54" s="34" t="str">
+        <f t="shared" si="37"/>
+        <v>FF0000F0</v>
+      </c>
+      <c r="J54" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="K54" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="L54" s="35" t="str">
+        <f t="shared" si="41"/>
+        <v>0xFF000030</v>
+      </c>
+      <c r="M54" s="35" t="str">
+        <f t="shared" si="42"/>
+        <v>FF000030</v>
+      </c>
+      <c r="N54" s="36">
+        <f t="shared" si="43"/>
+        <v>4278190128</v>
+      </c>
+      <c r="O54" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="P54" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_WAN_EGRESS="0xFF000030/0xFF0000F0"</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="34" t="str">
+        <f t="shared" si="8"/>
+        <v>FF</v>
+      </c>
+      <c r="C55" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="D55" s="34">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="E55" s="34">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="F55" s="34">
+        <f>$D$12</f>
+        <v>0</v>
+      </c>
+      <c r="G55" s="34">
+        <f>$D$20</f>
+        <v>4</v>
+      </c>
+      <c r="H55" s="34">
+        <f>$D$16</f>
+        <v>0</v>
+      </c>
+      <c r="I55" s="34" t="str">
+        <f t="shared" si="37"/>
+        <v>FF0000F0</v>
+      </c>
+      <c r="J55" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="K55" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="L55" s="35" t="str">
+        <f t="shared" si="41"/>
+        <v>0xFF000040</v>
+      </c>
+      <c r="M55" s="35" t="str">
+        <f t="shared" si="42"/>
+        <v>FF000040</v>
+      </c>
+      <c r="N55" s="36">
+        <f t="shared" si="43"/>
+        <v>4278190144</v>
+      </c>
+      <c r="O55" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="P55" s="28" t="str">
+        <f t="shared" si="19"/>
+        <v>MASK_TUN_EGRESS="0xFF000040/0xFF0000F0"</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug from previous commit. packet marks LAN-WAN and LAN-TUN
</commit_message>
<xml_diff>
--- a/CES_Packet_Mark.xlsx
+++ b/CES_Packet_Mark.xlsx
@@ -547,6 +547,33 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -567,33 +594,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -896,12 +896,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
@@ -916,7 +916,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="30" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -931,7 +931,7 @@
       </c>
     </row>
     <row r="5" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="17" t="s">
         <v>12</v>
       </c>
@@ -944,7 +944,7 @@
       </c>
     </row>
     <row r="6" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="34" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -959,7 +959,7 @@
       </c>
     </row>
     <row r="7" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="18" t="s">
         <v>13</v>
       </c>
@@ -972,7 +972,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="27"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="18" t="s">
         <v>14</v>
       </c>
@@ -985,7 +985,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="17" t="s">
@@ -1000,7 +1000,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="17" t="s">
         <v>16</v>
       </c>
@@ -1013,7 +1013,7 @@
       </c>
     </row>
     <row r="11" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="17" t="s">
         <v>15</v>
       </c>
@@ -1026,7 +1026,7 @@
       </c>
     </row>
     <row r="12" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="18" t="s">
@@ -1041,7 +1041,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="18" t="s">
         <v>16</v>
       </c>
@@ -1054,7 +1054,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
+      <c r="B14" s="35"/>
       <c r="C14" s="18" t="s">
         <v>17</v>
       </c>
@@ -1067,7 +1067,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="27"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="18" t="s">
         <v>18</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="17" t="s">
@@ -1095,7 +1095,7 @@
       </c>
     </row>
     <row r="17" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="17" t="s">
         <v>16</v>
       </c>
@@ -1108,7 +1108,7 @@
       </c>
     </row>
     <row r="18" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="17" t="s">
         <v>20</v>
       </c>
@@ -1121,7 +1121,7 @@
       </c>
     </row>
     <row r="19" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="17" t="s">
         <v>21</v>
       </c>
@@ -1134,7 +1134,7 @@
       </c>
     </row>
     <row r="20" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="23"/>
+      <c r="B20" s="32"/>
       <c r="C20" s="17" t="s">
         <v>22</v>
       </c>
@@ -1228,7 +1228,7 @@
       <c r="J23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K23" s="29" t="s">
+      <c r="K23" s="22" t="s">
         <v>50</v>
       </c>
       <c r="L23" s="2" t="str">
@@ -1246,9 +1246,9 @@
       <c r="O23" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P23" s="28" t="str">
-        <f>CONCATENATE(K23,"=",CHAR(34),L23,CHAR(34))</f>
-        <v>MARK_LOCAL_FROM_LAN="0xFF121212"</v>
+      <c r="P23" s="21" t="str">
+        <f>CONCATENATE(K23,"=",CHAR(34),L23,"/0x",I23,CHAR(34))</f>
+        <v>MARK_LOCAL_FROM_LAN="0xFF121212/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1286,7 +1286,7 @@
       <c r="J24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K24" s="29" t="s">
+      <c r="K24" s="22" t="s">
         <v>55</v>
       </c>
       <c r="L24" s="2" t="str">
@@ -1304,9 +1304,9 @@
       <c r="O24" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="P24" s="28" t="str">
-        <f t="shared" ref="P24:P32" si="5">CONCATENATE(K24,"=",CHAR(34),L24,CHAR(34))</f>
-        <v>MARK_LOCAL_TO_LAN="0xFF211221"</v>
+      <c r="P24" s="21" t="str">
+        <f t="shared" ref="P24:P32" si="5">CONCATENATE(K24,"=",CHAR(34),L24,"/0x",I24,CHAR(34))</f>
+        <v>MARK_LOCAL_TO_LAN="0xFF211221/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
       <c r="J25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K25" s="30" t="s">
+      <c r="K25" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L25" s="4" t="str">
@@ -1362,9 +1362,9 @@
       <c r="O25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P25" s="28" t="str">
+      <c r="P25" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>MARK_LOCAL_FROM_WAN="0xFF021113"</v>
+        <v>MARK_LOCAL_FROM_WAN="0xFF021113/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1402,7 +1402,7 @@
       <c r="J26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="30" t="s">
+      <c r="K26" s="23" t="s">
         <v>56</v>
       </c>
       <c r="L26" s="4" t="str">
@@ -1420,9 +1420,9 @@
       <c r="O26" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="P26" s="28" t="str">
+      <c r="P26" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>MARK_LOCAL_TO_WAN="0xFF011131"</v>
+        <v>MARK_LOCAL_TO_WAN="0xFF011131/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="27" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
       <c r="J27" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K27" s="31" t="s">
+      <c r="K27" s="24" t="s">
         <v>52</v>
       </c>
       <c r="L27" s="6" t="str">
@@ -1478,9 +1478,9 @@
       <c r="O27" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P27" s="28" t="str">
+      <c r="P27" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>MARK_LOCAL_FROM_TUN="0xFF021114"</v>
+        <v>MARK_LOCAL_FROM_TUN="0xFF021114/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
       <c r="J28" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K28" s="31" t="s">
+      <c r="K28" s="24" t="s">
         <v>57</v>
       </c>
       <c r="L28" s="6" t="str">
@@ -1536,9 +1536,9 @@
       <c r="O28" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="P28" s="28" t="str">
+      <c r="P28" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>MARK_LOCAL_TO_TUN="0xFF011141"</v>
+        <v>MARK_LOCAL_TO_TUN="0xFF011141/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="29" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1563,40 +1563,40 @@
         <v>2</v>
       </c>
       <c r="G29" s="8">
-        <f>$D$18</f>
-        <v>2</v>
-      </c>
-      <c r="H29" s="8">
         <f>$D$19</f>
         <v>3</v>
       </c>
+      <c r="H29" s="8">
+        <f>$D$18</f>
+        <v>2</v>
+      </c>
       <c r="I29" s="8" t="s">
         <v>89</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K29" s="32" t="s">
+      <c r="K29" s="25" t="s">
         <v>58</v>
       </c>
       <c r="L29" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>0xFF222223</v>
+        <v>0xFF222232</v>
       </c>
       <c r="M29" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>FF222223</v>
+        <v>FF222232</v>
       </c>
       <c r="N29" s="9">
         <f t="shared" si="4"/>
-        <v>4280427043</v>
+        <v>4280427058</v>
       </c>
       <c r="O29" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P29" s="28" t="str">
+      <c r="P29" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>MARK_LAN_TO_WAN="0xFF222223"</v>
+        <v>MARK_LAN_TO_WAN="0xFF222232/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="30" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1621,40 +1621,40 @@
         <v>2</v>
       </c>
       <c r="G30" s="8">
+        <f>$D$18</f>
+        <v>2</v>
+      </c>
+      <c r="H30" s="8">
         <f>$D$19</f>
         <v>3</v>
       </c>
-      <c r="H30" s="8">
-        <f>$D$18</f>
-        <v>2</v>
-      </c>
       <c r="I30" s="8" t="s">
         <v>89</v>
       </c>
       <c r="J30" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="K30" s="32" t="s">
+      <c r="K30" s="25" t="s">
         <v>53</v>
       </c>
       <c r="L30" s="8" t="str">
         <f t="shared" si="2"/>
-        <v>0xFF112232</v>
+        <v>0xFF112223</v>
       </c>
       <c r="M30" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>FF112232</v>
+        <v>FF112223</v>
       </c>
       <c r="N30" s="9">
         <f>HEX2DEC(M30)</f>
-        <v>4279312946</v>
+        <v>4279312931</v>
       </c>
       <c r="O30" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P30" s="28" t="str">
+      <c r="P30" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>MARK_LAN_FROM_WAN="0xFF112232"</v>
+        <v>MARK_LAN_FROM_WAN="0xFF112223/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="31" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1692,7 +1692,7 @@
       <c r="J31" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K31" s="33" t="s">
+      <c r="K31" s="26" t="s">
         <v>59</v>
       </c>
       <c r="L31" s="10" t="str">
@@ -1710,9 +1710,9 @@
       <c r="O31" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P31" s="28" t="str">
+      <c r="P31" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>MARK_LAN_TO_TUN="0xFF222342"</v>
+        <v>MARK_LAN_TO_TUN="0xFF222342/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="32" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1750,7 +1750,7 @@
       <c r="J32" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K32" s="33" t="s">
+      <c r="K32" s="26" t="s">
         <v>54</v>
       </c>
       <c r="L32" s="10" t="str">
@@ -1768,1030 +1768,1030 @@
       <c r="O32" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P32" s="28" t="str">
+      <c r="P32" s="21" t="str">
         <f t="shared" si="5"/>
-        <v>MARK_LAN_FROM_TUN="0xFF112324"</v>
+        <v>MARK_LAN_FROM_TUN="0xFF112324/0xFFFFFFFF"</v>
       </c>
     </row>
     <row r="33" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K33" s="28"/>
-      <c r="P33" s="28"/>
+      <c r="K33" s="21"/>
+      <c r="P33" s="21"/>
     </row>
     <row r="34" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K34" s="28"/>
-      <c r="P34" s="28"/>
+      <c r="K34" s="21"/>
+      <c r="P34" s="21"/>
     </row>
     <row r="35" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="34" t="str">
+      <c r="B35" s="27" t="str">
         <f t="shared" ref="B35:B55" si="8">$D$5</f>
         <v>FF</v>
       </c>
-      <c r="C35" s="34">
+      <c r="C35" s="27">
         <f t="shared" ref="C35:D40" si="9">$D$6</f>
         <v>0</v>
       </c>
-      <c r="D35" s="34">
+      <c r="D35" s="27">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="27">
         <f t="shared" ref="E35:E37" si="10">$D$10</f>
         <v>1</v>
       </c>
-      <c r="F35" s="34">
+      <c r="F35" s="27">
         <f>$D$12</f>
         <v>0</v>
       </c>
-      <c r="G35" s="34">
-        <f t="shared" ref="G35:H40" si="11">$D$17</f>
-        <v>1</v>
-      </c>
-      <c r="H35" s="34">
+      <c r="G35" s="27">
+        <f t="shared" ref="G35:H37" si="11">$D$17</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="I35" s="34" t="str">
+      <c r="I35" s="27" t="str">
         <f>CONCATENATE(IF(B35&lt;&gt;0,"FF","0"),IF(C35&lt;&gt;0,"F","0"),IF(D35&lt;&gt;0,"F","0"), IF(E35&lt;&gt;0,"F","0"),IF(F35&lt;&gt;0,"F","0"),IF(G35&lt;&gt;0,"F","0"), IF(H35&lt;&gt;0,"F","0"))</f>
         <v>FF00F0F0</v>
       </c>
-      <c r="J35" s="34" t="s">
+      <c r="J35" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="K35" s="34" t="s">
+      <c r="K35" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="L35" s="35" t="str">
+      <c r="L35" s="28" t="str">
         <f t="shared" ref="L35" si="12">CONCATENATE("0x",B35,C35,D35,E35,F35,G35,H35)</f>
         <v>0xFF001010</v>
       </c>
-      <c r="M35" s="35" t="str">
+      <c r="M35" s="28" t="str">
         <f t="shared" ref="M35" si="13">CONCATENATE(B35,C35,D35,E35,F35,G35,H35)</f>
         <v>FF001010</v>
       </c>
-      <c r="N35" s="36">
+      <c r="N35" s="29">
         <f>HEX2DEC(M35)</f>
         <v>4278194192</v>
       </c>
       <c r="O35" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="P35" s="28" t="str">
+      <c r="P35" s="21" t="str">
         <f>CONCATENATE(K35,"=",CHAR(34),L35,"/0x",I35,CHAR(34))</f>
         <v>MASK_LOCAL="0xFF001010/0xFF00F0F0"</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="34" t="str">
+      <c r="B36" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C36" s="34">
+      <c r="C36" s="27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="D36" s="34">
+      <c r="D36" s="27">
         <f>$D$8</f>
         <v>2</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="27">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="F36" s="34">
+      <c r="F36" s="27">
         <f>$D$12</f>
         <v>0</v>
       </c>
-      <c r="G36" s="34">
+      <c r="G36" s="27">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="H36" s="34">
+      <c r="H36" s="27">
         <f t="shared" ref="G36:H47" si="14">$D$16</f>
         <v>0</v>
       </c>
-      <c r="I36" s="34" t="str">
+      <c r="I36" s="27" t="str">
         <f t="shared" ref="I36:I37" si="15">CONCATENATE(IF(B36&lt;&gt;0,"FF","0"),IF(C36&lt;&gt;0,"F","0"),IF(D36&lt;&gt;0,"F","0"), IF(E36&lt;&gt;0,"F","0"),IF(F36&lt;&gt;0,"F","0"),IF(G36&lt;&gt;0,"F","0"), IF(H36&lt;&gt;0,"F","0"))</f>
         <v>FF0FF0F0</v>
       </c>
-      <c r="J36" s="34" t="s">
+      <c r="J36" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K36" s="34" t="s">
+      <c r="K36" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="L36" s="35" t="str">
+      <c r="L36" s="28" t="str">
         <f t="shared" ref="L36:L37" si="16">CONCATENATE("0x",B36,C36,D36,E36,F36,G36,H36)</f>
         <v>0xFF021010</v>
       </c>
-      <c r="M36" s="35" t="str">
+      <c r="M36" s="28" t="str">
         <f t="shared" ref="M36:M37" si="17">CONCATENATE(B36,C36,D36,E36,F36,G36,H36)</f>
         <v>FF021010</v>
       </c>
-      <c r="N36" s="36">
+      <c r="N36" s="29">
         <f t="shared" ref="N36:N37" si="18">HEX2DEC(M36)</f>
         <v>4278325264</v>
       </c>
       <c r="O36" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P36" s="28" t="str">
+      <c r="P36" s="21" t="str">
         <f t="shared" ref="P36:P55" si="19">CONCATENATE(K36,"=",CHAR(34),L36,"/0x",I36,CHAR(34))</f>
         <v>MASK_LOCAL_INGRESS="0xFF021010/0xFF0FF0F0"</v>
       </c>
     </row>
     <row r="37" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="34" t="str">
+      <c r="B37" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C37" s="34">
+      <c r="C37" s="27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="D37" s="34">
+      <c r="D37" s="27">
         <f>$D$7</f>
         <v>1</v>
       </c>
-      <c r="E37" s="34">
+      <c r="E37" s="27">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="F37" s="34">
+      <c r="F37" s="27">
         <f>$D$12</f>
         <v>0</v>
       </c>
-      <c r="G37" s="34">
+      <c r="G37" s="27">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H37" s="34">
+      <c r="H37" s="27">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="I37" s="34" t="str">
+      <c r="I37" s="27" t="str">
         <f t="shared" si="15"/>
         <v>FF0FF00F</v>
       </c>
-      <c r="J37" s="34" t="s">
+      <c r="J37" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="K37" s="34" t="s">
+      <c r="K37" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="L37" s="35" t="str">
+      <c r="L37" s="28" t="str">
         <f t="shared" si="16"/>
         <v>0xFF011001</v>
       </c>
-      <c r="M37" s="35" t="str">
+      <c r="M37" s="28" t="str">
         <f t="shared" si="17"/>
         <v>FF011001</v>
       </c>
-      <c r="N37" s="36">
+      <c r="N37" s="29">
         <f t="shared" si="18"/>
         <v>4278259713</v>
       </c>
       <c r="O37" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="P37" s="28" t="str">
+      <c r="P37" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_LOCAL_EGRESS="0xFF011001/0xFF0FF00F"</v>
       </c>
     </row>
     <row r="38" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P38" s="28"/>
+      <c r="P38" s="21"/>
     </row>
     <row r="39" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="34" t="str">
+      <c r="B39" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C39" s="34">
+      <c r="C39" s="27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="D39" s="34">
+      <c r="D39" s="27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E39" s="34">
+      <c r="E39" s="27">
         <f t="shared" ref="E39:E40" si="20">$D$9</f>
         <v>0</v>
       </c>
-      <c r="F39" s="34">
+      <c r="F39" s="27">
         <f>$D$12</f>
         <v>0</v>
       </c>
-      <c r="G39" s="34">
+      <c r="G39" s="27">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="H39" s="34">
+      <c r="H39" s="27">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="I39" s="34" t="str">
+      <c r="I39" s="27" t="str">
         <f t="shared" ref="I39:I40" si="21">CONCATENATE(IF(B39&lt;&gt;0,"FF","0"),IF(C39&lt;&gt;0,"F","0"),IF(D39&lt;&gt;0,"F","0"), IF(E39&lt;&gt;0,"F","0"),IF(F39&lt;&gt;0,"F","0"),IF(G39&lt;&gt;0,"F","0"), IF(H39&lt;&gt;0,"F","0"))</f>
         <v>FF0000F0</v>
       </c>
-      <c r="J39" s="34" t="s">
+      <c r="J39" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="K39" s="34" t="s">
+      <c r="K39" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="L39" s="35" t="str">
+      <c r="L39" s="28" t="str">
         <f>CONCATENATE("0x",B39,C39,D39,E39,F39,G39,H39)</f>
         <v>0xFF000020</v>
       </c>
-      <c r="M39" s="35" t="str">
+      <c r="M39" s="28" t="str">
         <f>CONCATENATE(B39,C39,D39,E39,F39,G39,H39)</f>
         <v>FF000020</v>
       </c>
-      <c r="N39" s="36">
+      <c r="N39" s="29">
         <f t="shared" ref="N39:N40" si="22">HEX2DEC(M39)</f>
         <v>4278190112</v>
       </c>
       <c r="O39" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P39" s="28" t="str">
+      <c r="P39" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_HOST_INGRESS="0xFF000020/0xFF0000F0"</v>
       </c>
     </row>
     <row r="40" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="34" t="str">
+      <c r="B40" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C40" s="34">
+      <c r="C40" s="27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="D40" s="34">
+      <c r="D40" s="27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="E40" s="34">
+      <c r="E40" s="27">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
-      <c r="F40" s="34">
+      <c r="F40" s="27">
         <f>$D$12</f>
         <v>0</v>
       </c>
-      <c r="G40" s="34">
+      <c r="G40" s="27">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="H40" s="34">
+      <c r="H40" s="27">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="I40" s="34" t="str">
+      <c r="I40" s="27" t="str">
         <f t="shared" si="21"/>
         <v>FF00000F</v>
       </c>
-      <c r="J40" s="34" t="s">
+      <c r="J40" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="K40" s="34" t="s">
+      <c r="K40" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="L40" s="35" t="str">
+      <c r="L40" s="28" t="str">
         <f>CONCATENATE("0x",B40,C40,D40,E40,F40,G40,H40)</f>
         <v>0xFF000002</v>
       </c>
-      <c r="M40" s="35" t="str">
+      <c r="M40" s="28" t="str">
         <f>CONCATENATE(B40,C40,D40,E40,F40,G40,H40)</f>
         <v>FF000002</v>
       </c>
-      <c r="N40" s="36">
+      <c r="N40" s="29">
         <f t="shared" si="22"/>
         <v>4278190082</v>
       </c>
       <c r="O40" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P40" s="28" t="str">
+      <c r="P40" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_HOST_EGRESS="0xFF000002/0xFF00000F"</v>
       </c>
     </row>
     <row r="41" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P41" s="28"/>
+      <c r="P41" s="21"/>
     </row>
     <row r="42" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="34" t="str">
+      <c r="B42" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C42" s="34">
+      <c r="C42" s="27">
         <f t="shared" ref="C42:D55" si="23">$D$6</f>
         <v>0</v>
       </c>
-      <c r="D42" s="34">
+      <c r="D42" s="27">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="27">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F42" s="34">
+      <c r="F42" s="27">
         <f>$D$14</f>
         <v>2</v>
       </c>
-      <c r="G42" s="34">
+      <c r="G42" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H42" s="34">
+      <c r="H42" s="27">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="I42" s="34" t="str">
+      <c r="I42" s="27" t="str">
         <f t="shared" ref="I42:I44" si="24">CONCATENATE(IF(B42&lt;&gt;0,"FF","0"),IF(C42&lt;&gt;0,"F","0"),IF(D42&lt;&gt;0,"F","0"), IF(E42&lt;&gt;0,"F","0"),IF(F42&lt;&gt;0,"F","0"),IF(G42&lt;&gt;0,"F","0"), IF(H42&lt;&gt;0,"F","0"))</f>
         <v>FF000F00</v>
       </c>
-      <c r="J42" s="34" t="s">
+      <c r="J42" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="K42" s="34" t="s">
+      <c r="K42" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="L42" s="35" t="str">
+      <c r="L42" s="28" t="str">
         <f t="shared" ref="L42" si="25">CONCATENATE("0x",B42,C42,D42,E42,F42,G42,H42)</f>
         <v>0xFF000200</v>
       </c>
-      <c r="M42" s="35" t="str">
+      <c r="M42" s="28" t="str">
         <f t="shared" ref="M42" si="26">CONCATENATE(B42,C42,D42,E42,F42,G42,H42)</f>
         <v>FF000200</v>
       </c>
-      <c r="N42" s="36">
+      <c r="N42" s="29">
         <f>HEX2DEC(M42)</f>
         <v>4278190592</v>
       </c>
       <c r="O42" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P42" s="28" t="str">
+      <c r="P42" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_HOST_LEGACY="0xFF000200/0xFF000F00"</v>
       </c>
     </row>
     <row r="43" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="34" t="str">
+      <c r="B43" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C43" s="34">
+      <c r="C43" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D43" s="34">
+      <c r="D43" s="27">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E43" s="34">
+      <c r="E43" s="27">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F43" s="34">
+      <c r="F43" s="27">
         <f>$D$14</f>
         <v>2</v>
       </c>
-      <c r="G43" s="34">
+      <c r="G43" s="27">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="H43" s="34">
+      <c r="H43" s="27">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="I43" s="34" t="str">
+      <c r="I43" s="27" t="str">
         <f t="shared" si="24"/>
         <v>FF000FF0</v>
       </c>
-      <c r="J43" s="34" t="s">
+      <c r="J43" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="K43" s="34" t="s">
+      <c r="K43" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="L43" s="35" t="str">
+      <c r="L43" s="28" t="str">
         <f t="shared" ref="L43:L44" si="27">CONCATENATE("0x",B43,C43,D43,E43,F43,G43,H43)</f>
         <v>0xFF000220</v>
       </c>
-      <c r="M43" s="35" t="str">
+      <c r="M43" s="28" t="str">
         <f t="shared" ref="M43:M44" si="28">CONCATENATE(B43,C43,D43,E43,F43,G43,H43)</f>
         <v>FF000220</v>
       </c>
-      <c r="N43" s="36">
+      <c r="N43" s="29">
         <f t="shared" ref="N43:N44" si="29">HEX2DEC(M43)</f>
         <v>4278190624</v>
       </c>
       <c r="O43" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P43" s="28" t="str">
+      <c r="P43" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_HOST_LEGACY_INGRESS="0xFF000220/0xFF000FF0"</v>
       </c>
     </row>
     <row r="44" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="34" t="str">
+      <c r="B44" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C44" s="34">
+      <c r="C44" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D44" s="34">
+      <c r="D44" s="27">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E44" s="34">
+      <c r="E44" s="27">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F44" s="34">
+      <c r="F44" s="27">
         <f>$D$14</f>
         <v>2</v>
       </c>
-      <c r="G44" s="34">
+      <c r="G44" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H44" s="34">
+      <c r="H44" s="27">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="I44" s="34" t="str">
+      <c r="I44" s="27" t="str">
         <f t="shared" si="24"/>
         <v>FF000F0F</v>
       </c>
-      <c r="J44" s="34" t="s">
+      <c r="J44" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="K44" s="34" t="s">
+      <c r="K44" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="L44" s="35" t="str">
+      <c r="L44" s="28" t="str">
         <f t="shared" si="27"/>
         <v>0xFF000202</v>
       </c>
-      <c r="M44" s="35" t="str">
+      <c r="M44" s="28" t="str">
         <f t="shared" si="28"/>
         <v>FF000202</v>
       </c>
-      <c r="N44" s="36">
+      <c r="N44" s="29">
         <f t="shared" si="29"/>
         <v>4278190594</v>
       </c>
       <c r="O44" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P44" s="28" t="str">
+      <c r="P44" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_HOST_LEGACY_EGRESS="0xFF000202/0xFF000F0F"</v>
       </c>
     </row>
     <row r="45" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P45" s="28"/>
+      <c r="P45" s="21"/>
     </row>
     <row r="46" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="34" t="str">
+      <c r="B46" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C46" s="34">
+      <c r="C46" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D46" s="34">
+      <c r="D46" s="27">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E46" s="34">
+      <c r="E46" s="27">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F46" s="34">
+      <c r="F46" s="27">
         <f>$D$15</f>
         <v>3</v>
       </c>
-      <c r="G46" s="34">
+      <c r="G46" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H46" s="34">
+      <c r="H46" s="27">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="I46" s="34" t="str">
+      <c r="I46" s="27" t="str">
         <f t="shared" ref="I46:I48" si="30">CONCATENATE(IF(B46&lt;&gt;0,"FF","0"),IF(C46&lt;&gt;0,"F","0"),IF(D46&lt;&gt;0,"F","0"), IF(E46&lt;&gt;0,"F","0"),IF(F46&lt;&gt;0,"F","0"),IF(G46&lt;&gt;0,"F","0"), IF(H46&lt;&gt;0,"F","0"))</f>
         <v>FF000F00</v>
       </c>
-      <c r="J46" s="34" t="s">
+      <c r="J46" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="K46" s="34" t="s">
+      <c r="K46" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="L46" s="35" t="str">
+      <c r="L46" s="28" t="str">
         <f t="shared" ref="L46" si="31">CONCATENATE("0x",B46,C46,D46,E46,F46,G46,H46)</f>
         <v>0xFF000300</v>
       </c>
-      <c r="M46" s="35" t="str">
+      <c r="M46" s="28" t="str">
         <f t="shared" ref="M46" si="32">CONCATENATE(B46,C46,D46,E46,F46,G46,H46)</f>
         <v>FF000300</v>
       </c>
-      <c r="N46" s="36">
+      <c r="N46" s="29">
         <f>HEX2DEC(M46)</f>
         <v>4278190848</v>
       </c>
       <c r="O46" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P46" s="28" t="str">
+      <c r="P46" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_HOST_CES="0xFF000300/0xFF000F00"</v>
       </c>
     </row>
     <row r="47" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="34" t="str">
+      <c r="B47" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C47" s="34">
+      <c r="C47" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D47" s="34">
+      <c r="D47" s="27">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E47" s="34">
+      <c r="E47" s="27">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F47" s="34">
+      <c r="F47" s="27">
         <f t="shared" ref="F47:F48" si="33">$D$15</f>
         <v>3</v>
       </c>
-      <c r="G47" s="34">
+      <c r="G47" s="27">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="H47" s="34">
+      <c r="H47" s="27">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="I47" s="34" t="str">
+      <c r="I47" s="27" t="str">
         <f t="shared" si="30"/>
         <v>FF000FF0</v>
       </c>
-      <c r="J47" s="34" t="s">
+      <c r="J47" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="K47" s="34" t="s">
+      <c r="K47" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="L47" s="35" t="str">
+      <c r="L47" s="28" t="str">
         <f t="shared" ref="L47:L48" si="34">CONCATENATE("0x",B47,C47,D47,E47,F47,G47,H47)</f>
         <v>0xFF000320</v>
       </c>
-      <c r="M47" s="35" t="str">
+      <c r="M47" s="28" t="str">
         <f t="shared" ref="M47:M48" si="35">CONCATENATE(B47,C47,D47,E47,F47,G47,H47)</f>
         <v>FF000320</v>
       </c>
-      <c r="N47" s="36">
+      <c r="N47" s="29">
         <f t="shared" ref="N47:N48" si="36">HEX2DEC(M47)</f>
         <v>4278190880</v>
       </c>
       <c r="O47" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P47" s="28" t="str">
+      <c r="P47" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_HOST_CES_INGRESS="0xFF000320/0xFF000FF0"</v>
       </c>
     </row>
     <row r="48" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="34" t="str">
+      <c r="B48" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C48" s="34">
+      <c r="C48" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D48" s="34">
+      <c r="D48" s="27">
         <f>$D$6</f>
         <v>0</v>
       </c>
-      <c r="E48" s="34">
+      <c r="E48" s="27">
         <f>$D$9</f>
         <v>0</v>
       </c>
-      <c r="F48" s="34">
+      <c r="F48" s="27">
         <f t="shared" si="33"/>
         <v>3</v>
       </c>
-      <c r="G48" s="34">
+      <c r="G48" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H48" s="34">
+      <c r="H48" s="27">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="I48" s="34" t="str">
+      <c r="I48" s="27" t="str">
         <f t="shared" si="30"/>
         <v>FF000F0F</v>
       </c>
-      <c r="J48" s="34" t="s">
+      <c r="J48" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="K48" s="34" t="s">
+      <c r="K48" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="L48" s="35" t="str">
+      <c r="L48" s="28" t="str">
         <f t="shared" si="34"/>
         <v>0xFF000302</v>
       </c>
-      <c r="M48" s="35" t="str">
+      <c r="M48" s="28" t="str">
         <f t="shared" si="35"/>
         <v>FF000302</v>
       </c>
-      <c r="N48" s="36">
+      <c r="N48" s="29">
         <f t="shared" si="36"/>
         <v>4278190850</v>
       </c>
       <c r="O48" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P48" s="28" t="str">
+      <c r="P48" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_HOST_CES_EGRESS="0xFF000302/0xFF000F0F"</v>
       </c>
     </row>
     <row r="49" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P49" s="28"/>
+      <c r="P49" s="21"/>
     </row>
     <row r="50" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="34" t="str">
+      <c r="B50" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C50" s="34">
+      <c r="C50" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D50" s="34">
+      <c r="D50" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="E50" s="34">
-        <f>$D$9</f>
-        <v>0</v>
-      </c>
-      <c r="F50" s="34">
-        <f>$D$12</f>
-        <v>0</v>
-      </c>
-      <c r="G50" s="34">
+      <c r="E50" s="27">
+        <f t="shared" ref="E50:E55" si="37">$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="F50" s="27">
+        <f t="shared" ref="F50:F55" si="38">$D$12</f>
+        <v>0</v>
+      </c>
+      <c r="G50" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H50" s="34">
+      <c r="H50" s="27">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="I50" s="34" t="str">
-        <f t="shared" ref="I50:I55" si="37">CONCATENATE(IF(B50&lt;&gt;0,"FF","0"),IF(C50&lt;&gt;0,"F","0"),IF(D50&lt;&gt;0,"F","0"), IF(E50&lt;&gt;0,"F","0"),IF(F50&lt;&gt;0,"F","0"),IF(G50&lt;&gt;0,"F","0"), IF(H50&lt;&gt;0,"F","0"))</f>
+      <c r="I50" s="27" t="str">
+        <f t="shared" ref="I50:I55" si="39">CONCATENATE(IF(B50&lt;&gt;0,"FF","0"),IF(C50&lt;&gt;0,"F","0"),IF(D50&lt;&gt;0,"F","0"), IF(E50&lt;&gt;0,"F","0"),IF(F50&lt;&gt;0,"F","0"),IF(G50&lt;&gt;0,"F","0"), IF(H50&lt;&gt;0,"F","0"))</f>
         <v>FF00000F</v>
       </c>
-      <c r="J50" s="34" t="s">
+      <c r="J50" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="K50" s="34" t="s">
+      <c r="K50" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="L50" s="35" t="str">
-        <f t="shared" ref="L50" si="38">CONCATENATE("0x",B50,C50,D50,E50,F50,G50,H50)</f>
+      <c r="L50" s="28" t="str">
+        <f t="shared" ref="L50" si="40">CONCATENATE("0x",B50,C50,D50,E50,F50,G50,H50)</f>
         <v>0xFF000002</v>
       </c>
-      <c r="M50" s="35" t="str">
-        <f t="shared" ref="M50" si="39">CONCATENATE(B50,C50,D50,E50,F50,G50,H50)</f>
+      <c r="M50" s="28" t="str">
+        <f t="shared" ref="M50" si="41">CONCATENATE(B50,C50,D50,E50,F50,G50,H50)</f>
         <v>FF000002</v>
       </c>
-      <c r="N50" s="36">
-        <f t="shared" ref="N50" si="40">HEX2DEC(M50)</f>
+      <c r="N50" s="29">
+        <f t="shared" ref="N50" si="42">HEX2DEC(M50)</f>
         <v>4278190082</v>
       </c>
       <c r="O50" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P50" s="28" t="str">
+      <c r="P50" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_LAN_INGRESS="0xFF000002/0xFF00000F"</v>
       </c>
     </row>
     <row r="51" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="34" t="str">
+      <c r="B51" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C51" s="34">
+      <c r="C51" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D51" s="34">
+      <c r="D51" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="E51" s="34">
-        <f>$D$9</f>
-        <v>0</v>
-      </c>
-      <c r="F51" s="34">
-        <f>$D$12</f>
-        <v>0</v>
-      </c>
-      <c r="G51" s="34">
+      <c r="E51" s="27">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="27">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="G51" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H51" s="34">
+      <c r="H51" s="27">
         <f>$D$19</f>
         <v>3</v>
       </c>
-      <c r="I51" s="34" t="str">
-        <f t="shared" si="37"/>
+      <c r="I51" s="27" t="str">
+        <f t="shared" si="39"/>
         <v>FF00000F</v>
       </c>
-      <c r="J51" s="34" t="s">
+      <c r="J51" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="K51" s="34" t="s">
+      <c r="K51" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="L51" s="35" t="str">
-        <f t="shared" ref="L51:L55" si="41">CONCATENATE("0x",B51,C51,D51,E51,F51,G51,H51)</f>
+      <c r="L51" s="28" t="str">
+        <f t="shared" ref="L51:L55" si="43">CONCATENATE("0x",B51,C51,D51,E51,F51,G51,H51)</f>
         <v>0xFF000003</v>
       </c>
-      <c r="M51" s="35" t="str">
-        <f t="shared" ref="M51:M55" si="42">CONCATENATE(B51,C51,D51,E51,F51,G51,H51)</f>
+      <c r="M51" s="28" t="str">
+        <f t="shared" ref="M51:M55" si="44">CONCATENATE(B51,C51,D51,E51,F51,G51,H51)</f>
         <v>FF000003</v>
       </c>
-      <c r="N51" s="36">
-        <f t="shared" ref="N51:N55" si="43">HEX2DEC(M51)</f>
+      <c r="N51" s="29">
+        <f t="shared" ref="N51:N55" si="45">HEX2DEC(M51)</f>
         <v>4278190083</v>
       </c>
       <c r="O51" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P51" s="28" t="str">
+      <c r="P51" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_WAN_INGRESS="0xFF000003/0xFF00000F"</v>
       </c>
     </row>
     <row r="52" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="34" t="str">
+      <c r="B52" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C52" s="34">
+      <c r="C52" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D52" s="34">
+      <c r="D52" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="E52" s="34">
-        <f>$D$9</f>
-        <v>0</v>
-      </c>
-      <c r="F52" s="34">
-        <f>$D$12</f>
-        <v>0</v>
-      </c>
-      <c r="G52" s="34">
+      <c r="E52" s="27">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="27">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="H52" s="34">
+      <c r="H52" s="27">
         <f>$D$20</f>
         <v>4</v>
       </c>
-      <c r="I52" s="34" t="str">
-        <f t="shared" si="37"/>
+      <c r="I52" s="27" t="str">
+        <f t="shared" si="39"/>
         <v>FF00000F</v>
       </c>
-      <c r="J52" s="34" t="s">
+      <c r="J52" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="K52" s="34" t="s">
+      <c r="K52" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="L52" s="35" t="str">
-        <f t="shared" si="41"/>
+      <c r="L52" s="28" t="str">
+        <f t="shared" si="43"/>
         <v>0xFF000004</v>
       </c>
-      <c r="M52" s="35" t="str">
-        <f t="shared" si="42"/>
+      <c r="M52" s="28" t="str">
+        <f t="shared" si="44"/>
         <v>FF000004</v>
       </c>
-      <c r="N52" s="36">
-        <f t="shared" si="43"/>
+      <c r="N52" s="29">
+        <f t="shared" si="45"/>
         <v>4278190084</v>
       </c>
       <c r="O52" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="P52" s="28" t="str">
+      <c r="P52" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_TUN_INGRESS="0xFF000004/0xFF00000F"</v>
       </c>
     </row>
     <row r="53" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="34" t="str">
+      <c r="B53" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C53" s="34">
+      <c r="C53" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D53" s="34">
+      <c r="D53" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="E53" s="34">
-        <f>$D$9</f>
-        <v>0</v>
-      </c>
-      <c r="F53" s="34">
-        <f>$D$12</f>
-        <v>0</v>
-      </c>
-      <c r="G53" s="34">
+      <c r="E53" s="27">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="27">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="G53" s="27">
         <f>$D$18</f>
         <v>2</v>
       </c>
-      <c r="H53" s="34">
+      <c r="H53" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="I53" s="34" t="str">
-        <f t="shared" si="37"/>
+      <c r="I53" s="27" t="str">
+        <f t="shared" si="39"/>
         <v>FF0000F0</v>
       </c>
-      <c r="J53" s="34" t="s">
+      <c r="J53" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="K53" s="34" t="s">
+      <c r="K53" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="L53" s="35" t="str">
-        <f t="shared" si="41"/>
+      <c r="L53" s="28" t="str">
+        <f t="shared" si="43"/>
         <v>0xFF000020</v>
       </c>
-      <c r="M53" s="35" t="str">
-        <f t="shared" si="42"/>
+      <c r="M53" s="28" t="str">
+        <f t="shared" si="44"/>
         <v>FF000020</v>
       </c>
-      <c r="N53" s="36">
-        <f t="shared" si="43"/>
+      <c r="N53" s="29">
+        <f t="shared" si="45"/>
         <v>4278190112</v>
       </c>
       <c r="O53" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="P53" s="28" t="str">
+      <c r="P53" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_LAN_EGRESS="0xFF000020/0xFF0000F0"</v>
       </c>
     </row>
     <row r="54" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="34" t="str">
+      <c r="B54" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C54" s="34">
+      <c r="C54" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D54" s="34">
+      <c r="D54" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="E54" s="34">
-        <f>$D$9</f>
-        <v>0</v>
-      </c>
-      <c r="F54" s="34">
-        <f>$D$12</f>
-        <v>0</v>
-      </c>
-      <c r="G54" s="34">
+      <c r="E54" s="27">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="27">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="G54" s="27">
         <f>$D$19</f>
         <v>3</v>
       </c>
-      <c r="H54" s="34">
+      <c r="H54" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="I54" s="34" t="str">
-        <f t="shared" si="37"/>
+      <c r="I54" s="27" t="str">
+        <f t="shared" si="39"/>
         <v>FF0000F0</v>
       </c>
-      <c r="J54" s="34" t="s">
+      <c r="J54" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="K54" s="34" t="s">
+      <c r="K54" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="L54" s="35" t="str">
-        <f t="shared" si="41"/>
+      <c r="L54" s="28" t="str">
+        <f t="shared" si="43"/>
         <v>0xFF000030</v>
       </c>
-      <c r="M54" s="35" t="str">
-        <f t="shared" si="42"/>
+      <c r="M54" s="28" t="str">
+        <f t="shared" si="44"/>
         <v>FF000030</v>
       </c>
-      <c r="N54" s="36">
-        <f t="shared" si="43"/>
+      <c r="N54" s="29">
+        <f t="shared" si="45"/>
         <v>4278190128</v>
       </c>
       <c r="O54" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="P54" s="28" t="str">
+      <c r="P54" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_WAN_EGRESS="0xFF000030/0xFF0000F0"</v>
       </c>
     </row>
     <row r="55" spans="2:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="34" t="str">
+      <c r="B55" s="27" t="str">
         <f t="shared" si="8"/>
         <v>FF</v>
       </c>
-      <c r="C55" s="34">
+      <c r="C55" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D55" s="34">
+      <c r="D55" s="27">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="E55" s="34">
-        <f>$D$9</f>
-        <v>0</v>
-      </c>
-      <c r="F55" s="34">
-        <f>$D$12</f>
-        <v>0</v>
-      </c>
-      <c r="G55" s="34">
+      <c r="E55" s="27">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="27">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="G55" s="27">
         <f>$D$20</f>
         <v>4</v>
       </c>
-      <c r="H55" s="34">
+      <c r="H55" s="27">
         <f>$D$16</f>
         <v>0</v>
       </c>
-      <c r="I55" s="34" t="str">
-        <f t="shared" si="37"/>
+      <c r="I55" s="27" t="str">
+        <f t="shared" si="39"/>
         <v>FF0000F0</v>
       </c>
-      <c r="J55" s="34" t="s">
+      <c r="J55" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="K55" s="34" t="s">
+      <c r="K55" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="L55" s="35" t="str">
-        <f t="shared" si="41"/>
+      <c r="L55" s="28" t="str">
+        <f t="shared" si="43"/>
         <v>0xFF000040</v>
       </c>
-      <c r="M55" s="35" t="str">
-        <f t="shared" si="42"/>
+      <c r="M55" s="28" t="str">
+        <f t="shared" si="44"/>
         <v>FF000040</v>
       </c>
-      <c r="N55" s="36">
-        <f t="shared" si="43"/>
+      <c r="N55" s="29">
+        <f t="shared" si="45"/>
         <v>4278190144</v>
       </c>
       <c r="O55" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="P55" s="28" t="str">
+      <c r="P55" s="21" t="str">
         <f t="shared" si="19"/>
         <v>MASK_TUN_EGRESS="0xFF000040/0xFF0000F0"</v>
       </c>

</xml_diff>